<commit_message>
LED packages filled in.
git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@20311 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/LEDs.xlsx
+++ b/Digikey/LEDs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Stephen Deiss\Gadgetron\Gadgets\Libraries\Parts\Digikey\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="28860" windowHeight="17520" tabRatio="609" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28860" windowHeight="17520" tabRatio="609" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="5" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="0603" sheetId="15" r:id="rId3"/>
     <sheet name="TH" sheetId="17" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3214" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3317" uniqueCount="694">
   <si>
     <t>ï»¿"Datasheets"</t>
   </si>
@@ -2089,6 +2094,21 @@
   </si>
   <si>
     <t>2012-0805</t>
+  </si>
+  <si>
+    <t>LEDSC125X200X120-2_HS</t>
+  </si>
+  <si>
+    <t>1608-0603</t>
+  </si>
+  <si>
+    <t>LEDSC80X160X65-2_HS</t>
+  </si>
+  <si>
+    <t>LEDRD250W50D400H640_HS</t>
+  </si>
+  <si>
+    <t>4x6-TH-LED</t>
   </si>
 </sst>
 </file>
@@ -2340,7 +2360,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2350,6 +2370,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2479,6 +2502,26 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2630,28 +2673,16 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2662,20 +2693,20 @@
     <sortCondition ref="A7:A44"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Target Value" dataDxfId="12"/>
-    <tableColumn id="9" name="Bright" dataDxfId="11"/>
-    <tableColumn id="10" name="Dominant Wavelength" dataDxfId="10"/>
-    <tableColumn id="11" name="Stock" dataDxfId="9"/>
-    <tableColumn id="6" name="Query" dataDxfId="8">
+    <tableColumn id="1" name="Target Value" dataDxfId="14"/>
+    <tableColumn id="9" name="Bright" dataDxfId="13"/>
+    <tableColumn id="10" name="Dominant Wavelength" dataDxfId="12"/>
+    <tableColumn id="11" name="Stock" dataDxfId="11"/>
+    <tableColumn id="6" name="Query" dataDxfId="10">
       <calculatedColumnFormula>CONCATENATE(Table4[[#This Row],[Target Value]],Table4[[#This Row],[Bright]],Table4[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="0805 Status" dataDxfId="7">
+    <tableColumn id="3" name="0805 Status" dataDxfId="9">
       <calculatedColumnFormula>VLOOKUP(Table4[[#This Row],[Query]],'0805'!$AC$1:'0805'!$AC$50,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="0603 Status" dataDxfId="6">
+    <tableColumn id="4" name="0603 Status" dataDxfId="8">
       <calculatedColumnFormula>VLOOKUP(Table4[[#This Row],[Query]],'0603'!$AD$1:'0603'!$AD$50,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="TH" dataDxfId="5">
+    <tableColumn id="12" name="TH" dataDxfId="7">
       <calculatedColumnFormula>VLOOKUP(Table4[[#This Row],[Query]],TH!$AD$1:'TH'!$AD$50,1,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2718,7 +2749,7 @@
     <tableColumn id="25" name="Mounting Type"/>
     <tableColumn id="26" name="Stock"/>
     <tableColumn id="27" name="Brightness"/>
-    <tableColumn id="42" name="Query" dataDxfId="4">
+    <tableColumn id="42" name="Query" dataDxfId="6">
       <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="39" name="Package"/>
@@ -2768,12 +2799,12 @@
     <tableColumn id="23" name="Size / Dimension"/>
     <tableColumn id="24" name="Height"/>
     <tableColumn id="25" name="Mounting Type"/>
-    <tableColumn id="43" name="Stock Color?" dataDxfId="3">
+    <tableColumn id="43" name="Stock Color?" dataDxfId="5">
       <calculatedColumnFormula>VLOOKUP(Table113[[#This Row],[Wavelength - Dominant]],Values!$C$11:$E$20,2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="26" name="Stock"/>
     <tableColumn id="27" name="Brightness"/>
-    <tableColumn id="42" name="Query" dataDxfId="2">
+    <tableColumn id="42" name="Query" dataDxfId="4">
       <calculatedColumnFormula>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="39" name="Package"/>
@@ -2817,12 +2848,12 @@
     <tableColumn id="23" name="Size / Dimension"/>
     <tableColumn id="24" name="Height"/>
     <tableColumn id="25" name="Mounting Type"/>
-    <tableColumn id="44" name="Target color?" dataDxfId="1">
+    <tableColumn id="44" name="Target color?" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP(Table1131415[[#This Row],[Color]],Values!$A$11:$E$20,4,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="48" name="Bright"/>
     <tableColumn id="45" name="Stock"/>
-    <tableColumn id="46" name="Query" dataDxfId="0">
+    <tableColumn id="46" name="Query" dataDxfId="2">
       <calculatedColumnFormula>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="47" name="Package"/>
@@ -3160,20 +3191,20 @@
       <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>36</v>
       </c>
@@ -3181,7 +3212,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -3189,7 +3220,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
@@ -3197,7 +3228,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -3223,7 +3254,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -3253,7 +3284,7 @@
         <v>OrangedimStock</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -3283,7 +3314,7 @@
         <v>BluebrightStock</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -3313,7 +3344,7 @@
         <v>GreendimStock</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -3343,7 +3374,7 @@
         <v>GreenbrightStock</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -3373,7 +3404,7 @@
         <v>ReddimStock</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -3403,7 +3434,7 @@
         <v>RedbrightStock</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -3433,7 +3464,7 @@
         <v>White, CoolbrightStock</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>158</v>
       </c>
@@ -3463,7 +3494,7 @@
         <v>YellowbrightStock</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>158</v>
       </c>
@@ -3493,7 +3524,7 @@
         <v>YellowdimStock</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -3525,12 +3556,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F11:H20">
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="STOCK">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="STOCK">
       <formula>NOT(ISERROR(SEARCH("STOCK",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="STOCK">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="STOCK">
       <formula>NOT(ISERROR(SEARCH("STOCK",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3551,37 +3582,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView topLeftCell="AA1" workbookViewId="0">
       <pane xSplit="30300" topLeftCell="AC1"/>
-      <selection activeCell="AE7" sqref="AE7"/>
+      <selection activeCell="AD17" sqref="AD17"/>
       <selection pane="topRight" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="4" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="3" max="4" width="21.375" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.625" customWidth="1"/>
+    <col min="9" max="9" width="14.625" customWidth="1"/>
+    <col min="10" max="10" width="16.875" customWidth="1"/>
+    <col min="12" max="12" width="19.375" customWidth="1"/>
+    <col min="13" max="13" width="11.875" customWidth="1"/>
+    <col min="15" max="15" width="18.875" customWidth="1"/>
+    <col min="16" max="16" width="11.875" customWidth="1"/>
     <col min="17" max="17" width="15.5" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="20" max="20" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.625" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" customWidth="1"/>
+    <col min="22" max="22" width="15.875" customWidth="1"/>
     <col min="23" max="23" width="23.5" customWidth="1"/>
-    <col min="24" max="24" width="17.33203125" customWidth="1"/>
-    <col min="26" max="26" width="23.6640625" customWidth="1"/>
+    <col min="24" max="24" width="17.375" customWidth="1"/>
+    <col min="26" max="26" width="23.625" customWidth="1"/>
+    <col min="30" max="30" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="16" thickBot="1">
+    <row r="1" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3679,7 +3711,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="16" thickTop="1">
+    <row r="2" spans="1:32" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -3762,11 +3794,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>Amber</v>
       </c>
+      <c r="AD2" t="s">
+        <v>689</v>
+      </c>
       <c r="AE2" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3849,11 +3884,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AD3" t="s">
+        <v>689</v>
+      </c>
       <c r="AE3" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -3942,11 +3980,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>OrangedimSTOCK</v>
       </c>
+      <c r="AD4" t="s">
+        <v>689</v>
+      </c>
       <c r="AE4" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -4035,11 +4076,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>BluebrightSTOCK</v>
       </c>
+      <c r="AD5" t="s">
+        <v>689</v>
+      </c>
       <c r="AE5" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -4125,11 +4169,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>Greenmedium</v>
       </c>
+      <c r="AD6" t="s">
+        <v>689</v>
+      </c>
       <c r="AE6" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -4218,11 +4265,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>GreendimSTOCK</v>
       </c>
+      <c r="AD7" t="s">
+        <v>689</v>
+      </c>
       <c r="AE7" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -4311,11 +4361,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>GreenbrightSTOCK</v>
       </c>
+      <c r="AD8" t="s">
+        <v>689</v>
+      </c>
       <c r="AE8" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -4401,11 +4454,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>Redmedium</v>
       </c>
+      <c r="AD9" t="s">
+        <v>689</v>
+      </c>
       <c r="AE9" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>126</v>
       </c>
@@ -4494,11 +4550,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>ReddimSTOCK</v>
       </c>
+      <c r="AD10" t="s">
+        <v>689</v>
+      </c>
       <c r="AE10" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -4587,11 +4646,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>RedbrightSTOCK</v>
       </c>
+      <c r="AD11" t="s">
+        <v>689</v>
+      </c>
       <c r="AE11" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -4677,11 +4739,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>Redmedium</v>
       </c>
+      <c r="AD12" t="s">
+        <v>689</v>
+      </c>
       <c r="AE12" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -4767,11 +4832,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>Redmedium</v>
       </c>
+      <c r="AD13" t="s">
+        <v>689</v>
+      </c>
       <c r="AE13" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -4860,11 +4928,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>White, CoolbrightSTOCK</v>
       </c>
+      <c r="AD14" t="s">
+        <v>689</v>
+      </c>
       <c r="AE14" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -4953,11 +5024,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>YellowbrightSTOCK</v>
       </c>
+      <c r="AD15" t="s">
+        <v>689</v>
+      </c>
       <c r="AE15" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>162</v>
       </c>
@@ -5046,11 +5120,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>YellowdimSTOCK</v>
       </c>
+      <c r="AD16" t="s">
+        <v>689</v>
+      </c>
       <c r="AE16" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>166</v>
       </c>
@@ -5138,6 +5215,9 @@
       <c r="AC17" t="str">
         <f>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</f>
         <v>OrangebrightSTOCK</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>689</v>
       </c>
       <c r="AE17" t="s">
         <v>688</v>
@@ -5146,9 +5226,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5162,37 +5242,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG46"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane xSplit="14280" topLeftCell="AB1" activePane="topRight"/>
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <pane xSplit="14280" topLeftCell="AB1"/>
+      <selection activeCell="AE47" sqref="AE47:AE48"/>
       <selection pane="topRight" activeCell="AF5" sqref="AF5:AF46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="4" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="3" max="4" width="21.375" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
-    <col min="9" max="10" width="4.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="4.625" customWidth="1"/>
+    <col min="9" max="10" width="4.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" customWidth="1"/>
-    <col min="13" max="13" width="3.83203125" customWidth="1"/>
+    <col min="12" max="12" width="12.875" customWidth="1"/>
+    <col min="13" max="13" width="3.875" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" customWidth="1"/>
+    <col min="16" max="16" width="11.875" customWidth="1"/>
     <col min="17" max="17" width="15.5" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="20" max="20" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.625" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" customWidth="1"/>
+    <col min="22" max="22" width="15.875" customWidth="1"/>
     <col min="23" max="23" width="23.5" customWidth="1"/>
-    <col min="24" max="24" width="17.33203125" customWidth="1"/>
-    <col min="26" max="27" width="23.6640625" customWidth="1"/>
+    <col min="24" max="24" width="17.375" customWidth="1"/>
+    <col min="26" max="27" width="23.625" customWidth="1"/>
+    <col min="31" max="31" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="16" thickBot="1">
+    <row r="1" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5293,7 +5374,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:33" hidden="1">
+    <row r="2" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -5377,7 +5458,7 @@
         <v>Amber</v>
       </c>
     </row>
-    <row r="3" spans="1:33" hidden="1">
+    <row r="3" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>175</v>
       </c>
@@ -5465,7 +5546,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="4" spans="1:33" hidden="1">
+    <row r="4" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -5553,7 +5634,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="16" thickTop="1">
+    <row r="5" spans="1:33" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>268</v>
       </c>
@@ -5646,11 +5727,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>BluedimStock</v>
       </c>
+      <c r="AE5" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF5" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -5743,11 +5827,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>GreendimStock</v>
       </c>
+      <c r="AE6" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF6" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="7" spans="1:33" hidden="1">
+    <row r="7" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>226</v>
       </c>
@@ -5835,7 +5922,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="8" spans="1:33" hidden="1">
+    <row r="8" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>203</v>
       </c>
@@ -5923,7 +6010,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="9" spans="1:33" hidden="1">
+    <row r="9" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>208</v>
       </c>
@@ -6011,7 +6098,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -6104,11 +6191,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>GreenbrightStock</v>
       </c>
+      <c r="AE10" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF10" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="11" spans="1:33" hidden="1">
+    <row r="11" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>283</v>
       </c>
@@ -6196,7 +6286,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="12" spans="1:33" hidden="1">
+    <row r="12" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>339</v>
       </c>
@@ -6284,7 +6374,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>187</v>
       </c>
@@ -6377,11 +6467,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>OrangebrightStock</v>
       </c>
+      <c r="AE13" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF13" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>222</v>
       </c>
@@ -6474,11 +6567,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>OrangedimStock</v>
       </c>
+      <c r="AE14" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF14" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="15" spans="1:33" hidden="1">
+    <row r="15" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -6566,7 +6662,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="16" spans="1:33" hidden="1">
+    <row r="16" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>234</v>
       </c>
@@ -6654,7 +6750,7 @@
         <v>Blue</v>
       </c>
     </row>
-    <row r="17" spans="1:32" hidden="1">
+    <row r="17" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>240</v>
       </c>
@@ -6742,7 +6838,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="18" spans="1:32" hidden="1">
+    <row r="18" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>250</v>
       </c>
@@ -6830,7 +6926,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="19" spans="1:32" hidden="1">
+    <row r="19" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>255</v>
       </c>
@@ -6918,7 +7014,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="20" spans="1:32" hidden="1">
+    <row r="20" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>260</v>
       </c>
@@ -7006,7 +7102,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="21" spans="1:32" hidden="1">
+    <row r="21" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>265</v>
       </c>
@@ -7094,7 +7190,7 @@
         <v>Blue</v>
       </c>
     </row>
-    <row r="22" spans="1:32" hidden="1">
+    <row r="22" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>306</v>
       </c>
@@ -7182,7 +7278,7 @@
         <v>Orange</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>274</v>
       </c>
@@ -7275,11 +7371,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>BluebrightStock</v>
       </c>
+      <c r="AE23" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF23" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="24" spans="1:32" hidden="1">
+    <row r="24" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>318</v>
       </c>
@@ -7367,7 +7466,7 @@
         <v>Orange</v>
       </c>
     </row>
-    <row r="25" spans="1:32" hidden="1">
+    <row r="25" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>327</v>
       </c>
@@ -7455,7 +7554,7 @@
         <v>Orange</v>
       </c>
     </row>
-    <row r="26" spans="1:32" hidden="1">
+    <row r="26" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>286</v>
       </c>
@@ -7543,7 +7642,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>291</v>
       </c>
@@ -7636,11 +7735,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>White, CoolbrightStock</v>
       </c>
+      <c r="AE27" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF27" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="28" spans="1:32" hidden="1">
+    <row r="28" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>299</v>
       </c>
@@ -7728,7 +7830,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="29" spans="1:32">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>211</v>
       </c>
@@ -7821,11 +7923,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>ReddimStock</v>
       </c>
+      <c r="AE29" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF29" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="30" spans="1:32">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>311</v>
       </c>
@@ -7918,11 +8023,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>RedbrightStock</v>
       </c>
+      <c r="AE30" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF30" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="31" spans="1:32">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>194</v>
       </c>
@@ -8015,11 +8123,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>YellowbrightStock</v>
       </c>
+      <c r="AE31" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF31" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="32" spans="1:32" hidden="1">
+    <row r="32" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>215</v>
       </c>
@@ -8107,7 +8218,7 @@
         <v>Yellow</v>
       </c>
     </row>
-    <row r="33" spans="1:33" hidden="1">
+    <row r="33" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>323</v>
       </c>
@@ -8195,7 +8306,7 @@
         <v>Yellow</v>
       </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>219</v>
       </c>
@@ -8288,11 +8399,14 @@
         <f>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</f>
         <v>YellowdimStock</v>
       </c>
+      <c r="AE34" s="9" t="s">
+        <v>691</v>
+      </c>
       <c r="AF34" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
-    <row r="35" spans="1:33" hidden="1">
+    <row r="35" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>331</v>
       </c>
@@ -8380,7 +8494,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="36" spans="1:33" hidden="1">
+    <row r="36" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>314</v>
       </c>
@@ -8468,7 +8582,7 @@
         <v>Yellow</v>
       </c>
     </row>
-    <row r="37" spans="1:33" hidden="1">
+    <row r="37" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>342</v>
       </c>
@@ -8556,7 +8670,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="38" spans="1:33" hidden="1">
+    <row r="38" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>347</v>
       </c>
@@ -8640,7 +8754,7 @@
         <v>Amber</v>
       </c>
     </row>
-    <row r="39" spans="1:33" hidden="1">
+    <row r="39" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>351</v>
       </c>
@@ -8724,7 +8838,7 @@
         <v>Amber</v>
       </c>
     </row>
-    <row r="40" spans="1:33" hidden="1">
+    <row r="40" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>211</v>
       </c>
@@ -8808,7 +8922,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="41" spans="1:33" hidden="1">
+    <row r="41" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>359</v>
       </c>
@@ -8892,7 +9006,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="42" spans="1:33" hidden="1">
+    <row r="42" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>362</v>
       </c>
@@ -8976,7 +9090,7 @@
         <v>Blue</v>
       </c>
     </row>
-    <row r="43" spans="1:33" hidden="1">
+    <row r="43" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>367</v>
       </c>
@@ -9060,7 +9174,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="44" spans="1:33" hidden="1">
+    <row r="44" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>373</v>
       </c>
@@ -9144,7 +9258,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="45" spans="1:33" hidden="1">
+    <row r="45" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>381</v>
       </c>
@@ -9228,7 +9342,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="46" spans="1:33" hidden="1">
+    <row r="46" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>386</v>
       </c>
@@ -9321,9 +9435,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -9337,37 +9451,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF77"/>
   <sheetViews>
-    <sheetView topLeftCell="W45" workbookViewId="0">
-      <pane xSplit="14340" topLeftCell="AC1" activePane="topRight"/>
-      <selection activeCell="P90" sqref="P90"/>
-      <selection pane="topRight" activeCell="AF79" sqref="AF79"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="4" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="3" max="4" width="21.375" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
-    <col min="9" max="10" width="4.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.75" customWidth="1"/>
+    <col min="7" max="7" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="4.625" customWidth="1"/>
+    <col min="9" max="10" width="4.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" customWidth="1"/>
-    <col min="13" max="13" width="3.83203125" customWidth="1"/>
+    <col min="12" max="12" width="12.875" customWidth="1"/>
+    <col min="13" max="13" width="15.125" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" customWidth="1"/>
+    <col min="16" max="16" width="11.875" customWidth="1"/>
     <col min="17" max="17" width="15.5" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="20" max="20" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.625" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" customWidth="1"/>
+    <col min="22" max="22" width="15.875" customWidth="1"/>
     <col min="23" max="23" width="23.5" customWidth="1"/>
-    <col min="24" max="24" width="17.33203125" customWidth="1"/>
-    <col min="26" max="26" width="23.6640625" customWidth="1"/>
+    <col min="24" max="24" width="17.375" customWidth="1"/>
+    <col min="26" max="26" width="23.625" customWidth="1"/>
+    <col min="31" max="31" width="32.75" customWidth="1"/>
+    <col min="32" max="32" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="16" thickBot="1">
+    <row r="1" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9465,7 +9579,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="16" thickTop="1">
+    <row r="2" spans="1:32" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>455</v>
       </c>
@@ -9558,11 +9672,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>BluebrightStock</v>
       </c>
+      <c r="AE2" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF2" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>405</v>
       </c>
@@ -9649,11 +9766,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE3" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF3" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>405</v>
       </c>
@@ -9740,11 +9860,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE4" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF4" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>405</v>
       </c>
@@ -9831,11 +9954,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE5" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF5" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>405</v>
       </c>
@@ -9922,11 +10048,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE6" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF6" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>405</v>
       </c>
@@ -10013,11 +10142,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE7" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF7" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>455</v>
       </c>
@@ -10104,11 +10236,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Blue</v>
       </c>
+      <c r="AE8" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF8" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>397</v>
       </c>
@@ -10201,11 +10336,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>GreendimStock</v>
       </c>
+      <c r="AE9" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF9" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>397</v>
       </c>
@@ -10292,11 +10430,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE10" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF10" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>447</v>
       </c>
@@ -10389,11 +10530,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>GreenbrightStock</v>
       </c>
+      <c r="AE11" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF11" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>405</v>
       </c>
@@ -10480,11 +10624,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE12" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF12" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>442</v>
       </c>
@@ -10571,11 +10718,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE13" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF13" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>442</v>
       </c>
@@ -10662,11 +10812,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE14" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF14" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>397</v>
       </c>
@@ -10753,11 +10906,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE15" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF15" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>442</v>
       </c>
@@ -10850,11 +11006,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>OrangedimStock</v>
       </c>
+      <c r="AE16" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF16" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>397</v>
       </c>
@@ -10947,11 +11106,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>OrangebrightStock</v>
       </c>
+      <c r="AE17" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF17" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>455</v>
       </c>
@@ -11038,11 +11200,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Blue-Green</v>
       </c>
+      <c r="AE18" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF18" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>442</v>
       </c>
@@ -11129,11 +11294,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE19" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF19" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -11220,11 +11388,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE20" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF20" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>397</v>
       </c>
@@ -11317,11 +11488,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>ReddimStock</v>
       </c>
+      <c r="AE21" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF21" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>397</v>
       </c>
@@ -11408,11 +11582,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE22" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF22" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>442</v>
       </c>
@@ -11499,11 +11676,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE23" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF23" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>442</v>
       </c>
@@ -11590,11 +11770,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE24" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF24" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>489</v>
       </c>
@@ -11681,11 +11864,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE25" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF25" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="26" spans="1:32">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>489</v>
       </c>
@@ -11778,11 +11964,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>RedbrightStock</v>
       </c>
+      <c r="AE26" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF26" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>502</v>
       </c>
@@ -11869,11 +12058,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>White, Cool</v>
       </c>
+      <c r="AE27" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF27" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="28" spans="1:32">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>455</v>
       </c>
@@ -11966,11 +12158,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>White, CoolbrightStock</v>
       </c>
+      <c r="AE28" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF28" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="29" spans="1:32">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>455</v>
       </c>
@@ -12057,11 +12252,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>White, Cool</v>
       </c>
+      <c r="AE29" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF29" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="30" spans="1:32">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>502</v>
       </c>
@@ -12148,11 +12346,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>White, Cool</v>
       </c>
+      <c r="AE30" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF30" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="31" spans="1:32">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>397</v>
       </c>
@@ -12245,11 +12446,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>YellowdimStock</v>
       </c>
+      <c r="AE31" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF31" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="32" spans="1:32">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>397</v>
       </c>
@@ -12336,11 +12540,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE32" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF32" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="33" spans="1:32">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>442</v>
       </c>
@@ -12427,11 +12634,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE33" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF33" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="34" spans="1:32">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>489</v>
       </c>
@@ -12524,11 +12734,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>YellowbrightStock</v>
       </c>
+      <c r="AE34" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF34" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="35" spans="1:32">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>455</v>
       </c>
@@ -12615,11 +12828,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Blue-Green</v>
       </c>
+      <c r="AE35" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF35" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="36" spans="1:32">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>541</v>
       </c>
@@ -12706,11 +12922,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE36" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF36" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="37" spans="1:32">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>541</v>
       </c>
@@ -12797,11 +13016,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE37" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF37" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="38" spans="1:32">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>541</v>
       </c>
@@ -12888,11 +13110,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE38" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF38" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="39" spans="1:32">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>541</v>
       </c>
@@ -12979,11 +13204,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE39" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF39" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="40" spans="1:32">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>541</v>
       </c>
@@ -13070,11 +13298,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE40" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF40" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="41" spans="1:32">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>541</v>
       </c>
@@ -13161,11 +13392,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE41" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF41" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="42" spans="1:32">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>541</v>
       </c>
@@ -13252,11 +13486,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE42" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF42" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="43" spans="1:32">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>541</v>
       </c>
@@ -13343,11 +13580,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE43" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF43" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="44" spans="1:32">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>541</v>
       </c>
@@ -13434,11 +13674,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE44" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF44" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="45" spans="1:32">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>442</v>
       </c>
@@ -13525,11 +13768,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE45" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF45" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="46" spans="1:32">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>541</v>
       </c>
@@ -13616,11 +13862,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE46" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF46" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="47" spans="1:32">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>541</v>
       </c>
@@ -13707,11 +13956,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE47" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF47" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="48" spans="1:32">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -13798,11 +14050,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE48" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF48" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="49" spans="1:32">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>589</v>
       </c>
@@ -13889,11 +14144,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE49" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF49" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="50" spans="1:32">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -13980,11 +14238,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE50" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF50" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="51" spans="1:32">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>405</v>
       </c>
@@ -14071,11 +14332,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE51" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF51" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="52" spans="1:32">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -14162,11 +14426,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE52" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF52" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="53" spans="1:32">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>405</v>
       </c>
@@ -14253,11 +14520,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE53" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF53" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="54" spans="1:32">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -14344,11 +14614,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE54" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF54" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="55" spans="1:32">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>405</v>
       </c>
@@ -14435,11 +14708,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE55" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF55" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="56" spans="1:32">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>589</v>
       </c>
@@ -14526,11 +14802,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE56" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF56" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="57" spans="1:32">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>489</v>
       </c>
@@ -14617,11 +14896,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE57" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF57" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="58" spans="1:32">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -14708,11 +14990,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE58" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF58" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="59" spans="1:32">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -14799,11 +15084,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE59" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF59" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="60" spans="1:32">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -14890,11 +15178,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE60" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF60" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="61" spans="1:32">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -14981,11 +15272,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE61" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF61" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="62" spans="1:32">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -15072,11 +15366,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE62" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF62" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="63" spans="1:32">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -15163,11 +15460,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE63" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF63" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="64" spans="1:32">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>405</v>
       </c>
@@ -15254,11 +15554,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE64" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF64" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="65" spans="1:32">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>489</v>
       </c>
@@ -15345,11 +15648,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE65" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF65" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="66" spans="1:32">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>649</v>
       </c>
@@ -15436,11 +15742,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Red</v>
       </c>
+      <c r="AE66" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF66" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="67" spans="1:32">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>489</v>
       </c>
@@ -15527,11 +15836,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Orange</v>
       </c>
+      <c r="AE67" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF67" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="68" spans="1:32">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>489</v>
       </c>
@@ -15618,11 +15930,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Yellow</v>
       </c>
+      <c r="AE68" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF68" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="69" spans="1:32">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>455</v>
       </c>
@@ -15709,11 +16024,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Blue</v>
       </c>
+      <c r="AE69" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF69" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="70" spans="1:32">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>455</v>
       </c>
@@ -15800,11 +16118,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Blue</v>
       </c>
+      <c r="AE70" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF70" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="71" spans="1:32">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>502</v>
       </c>
@@ -15891,11 +16212,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>White</v>
       </c>
+      <c r="AE71" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF71" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="72" spans="1:32">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>455</v>
       </c>
@@ -15982,11 +16306,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Blue</v>
       </c>
+      <c r="AE72" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF72" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="73" spans="1:32">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>17</v>
       </c>
@@ -16073,11 +16400,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>White</v>
       </c>
+      <c r="AE73" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF73" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="74" spans="1:32">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -16164,11 +16494,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>White</v>
       </c>
+      <c r="AE74" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF74" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="75" spans="1:32">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>677</v>
       </c>
@@ -16255,11 +16588,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Blue</v>
       </c>
+      <c r="AE75" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF75" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="76" spans="1:32">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>677</v>
       </c>
@@ -16346,11 +16682,14 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>Green</v>
       </c>
+      <c r="AE76" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF76" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
-    <row r="77" spans="1:32">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>502</v>
       </c>
@@ -16437,16 +16776,19 @@
         <f>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</f>
         <v>White, Cool</v>
       </c>
+      <c r="AE77" s="9" t="s">
+        <v>692</v>
+      </c>
       <c r="AF77" s="5" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
The libraries are in place for Koala, thanks mostly to Stephen Deiss.
Generating the CSV file for the parts database is very error-prone. 



git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@20390 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/LEDs.xlsx
+++ b/Digikey/LEDs.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Stephen Deiss\Gadgetron\Gadgets\Libraries\Parts\Digikey\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28860" windowHeight="17520" tabRatio="609" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25540" windowHeight="31460" tabRatio="609" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="5" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="0603" sheetId="15" r:id="rId3"/>
     <sheet name="TH" sheetId="17" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3317" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3317" uniqueCount="695">
   <si>
     <t>ï»¿"Datasheets"</t>
   </si>
@@ -2093,15 +2088,9 @@
     <t>Device</t>
   </si>
   <si>
-    <t>2012-0805</t>
-  </si>
-  <si>
     <t>LEDSC125X200X120-2_HS</t>
   </si>
   <si>
-    <t>1608-0603</t>
-  </si>
-  <si>
     <t>LEDSC80X160X65-2_HS</t>
   </si>
   <si>
@@ -2109,6 +2098,15 @@
   </si>
   <si>
     <t>4x6-TH-LED</t>
+  </si>
+  <si>
+    <t>SMD-1608-0603</t>
+  </si>
+  <si>
+    <t>TH-ROHM-4X6-ROUND</t>
+  </si>
+  <si>
+    <t>SMD-2012-0805</t>
   </si>
 </sst>
 </file>
@@ -2233,8 +2231,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2374,7 +2374,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="127">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2437,6 +2437,7 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2499,29 +2500,10 @@
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2673,6 +2655,26 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
@@ -2693,20 +2695,20 @@
     <sortCondition ref="A7:A44"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Target Value" dataDxfId="14"/>
-    <tableColumn id="9" name="Bright" dataDxfId="13"/>
-    <tableColumn id="10" name="Dominant Wavelength" dataDxfId="12"/>
-    <tableColumn id="11" name="Stock" dataDxfId="11"/>
-    <tableColumn id="6" name="Query" dataDxfId="10">
+    <tableColumn id="1" name="Target Value" dataDxfId="12"/>
+    <tableColumn id="9" name="Bright" dataDxfId="11"/>
+    <tableColumn id="10" name="Dominant Wavelength" dataDxfId="10"/>
+    <tableColumn id="11" name="Stock" dataDxfId="9"/>
+    <tableColumn id="6" name="Query" dataDxfId="8">
       <calculatedColumnFormula>CONCATENATE(Table4[[#This Row],[Target Value]],Table4[[#This Row],[Bright]],Table4[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="0805 Status" dataDxfId="9">
+    <tableColumn id="3" name="0805 Status" dataDxfId="7">
       <calculatedColumnFormula>VLOOKUP(Table4[[#This Row],[Query]],'0805'!$AC$1:'0805'!$AC$50,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="0603 Status" dataDxfId="8">
+    <tableColumn id="4" name="0603 Status" dataDxfId="6">
       <calculatedColumnFormula>VLOOKUP(Table4[[#This Row],[Query]],'0603'!$AD$1:'0603'!$AD$50,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="TH" dataDxfId="7">
+    <tableColumn id="12" name="TH" dataDxfId="5">
       <calculatedColumnFormula>VLOOKUP(Table4[[#This Row],[Query]],TH!$AD$1:'TH'!$AD$50,1,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2749,7 +2751,7 @@
     <tableColumn id="25" name="Mounting Type"/>
     <tableColumn id="26" name="Stock"/>
     <tableColumn id="27" name="Brightness"/>
-    <tableColumn id="42" name="Query" dataDxfId="6">
+    <tableColumn id="42" name="Query" dataDxfId="4">
       <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Color]],Table1[[#This Row],[Brightness]],Table1[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="39" name="Package"/>
@@ -2799,12 +2801,12 @@
     <tableColumn id="23" name="Size / Dimension"/>
     <tableColumn id="24" name="Height"/>
     <tableColumn id="25" name="Mounting Type"/>
-    <tableColumn id="43" name="Stock Color?" dataDxfId="5">
+    <tableColumn id="43" name="Stock Color?" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP(Table113[[#This Row],[Wavelength - Dominant]],Values!$C$11:$E$20,2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="26" name="Stock"/>
     <tableColumn id="27" name="Brightness"/>
-    <tableColumn id="42" name="Query" dataDxfId="4">
+    <tableColumn id="42" name="Query" dataDxfId="2">
       <calculatedColumnFormula>CONCATENATE(Table113[[#This Row],[Color]],Table113[[#This Row],[Brightness]],Table113[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="39" name="Package"/>
@@ -2817,7 +2819,13 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1131415" displayName="Table1131415" ref="A1:AF77" totalsRowShown="0">
-  <autoFilter ref="A1:AF77"/>
+  <autoFilter ref="A1:AF77">
+    <filterColumn colId="28">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:AE34">
     <sortCondition ref="N1:N77"/>
   </sortState>
@@ -2848,12 +2856,12 @@
     <tableColumn id="23" name="Size / Dimension"/>
     <tableColumn id="24" name="Height"/>
     <tableColumn id="25" name="Mounting Type"/>
-    <tableColumn id="44" name="Target color?" dataDxfId="3">
+    <tableColumn id="44" name="Target color?" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(Table1131415[[#This Row],[Color]],Values!$A$11:$E$20,4,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="48" name="Bright"/>
     <tableColumn id="45" name="Stock"/>
-    <tableColumn id="46" name="Query" dataDxfId="2">
+    <tableColumn id="46" name="Query" dataDxfId="0">
       <calculatedColumnFormula>CONCATENATE(Table1131415[[#This Row],[Color]],Table1131415[[#This Row],[Bright]],Table1131415[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="47" name="Package"/>
@@ -3191,20 +3199,20 @@
       <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="5" width="13.375" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>36</v>
       </c>
@@ -3212,7 +3220,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -3220,7 +3228,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
@@ -3228,7 +3236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -3254,7 +3262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -3284,7 +3292,7 @@
         <v>OrangedimStock</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -3314,7 +3322,7 @@
         <v>BluebrightStock</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -3344,7 +3352,7 @@
         <v>GreendimStock</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -3374,7 +3382,7 @@
         <v>GreenbrightStock</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -3404,7 +3412,7 @@
         <v>ReddimStock</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -3434,7 +3442,7 @@
         <v>RedbrightStock</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -3464,7 +3472,7 @@
         <v>White, CoolbrightStock</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>158</v>
       </c>
@@ -3494,7 +3502,7 @@
         <v>YellowbrightStock</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>158</v>
       </c>
@@ -3524,7 +3532,7 @@
         <v>YellowdimStock</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -3556,12 +3564,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F11:H20">
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="STOCK">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="STOCK">
       <formula>NOT(ISERROR(SEARCH("STOCK",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="STOCK">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="STOCK">
       <formula>NOT(ISERROR(SEARCH("STOCK",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3582,38 +3590,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
       <pane xSplit="30300" topLeftCell="AC1"/>
       <selection activeCell="AD17" sqref="AD17"/>
-      <selection pane="topRight" activeCell="AE1" sqref="AE1"/>
+      <selection pane="topRight" activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="3" max="4" width="21.375" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="3" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.625" customWidth="1"/>
-    <col min="9" max="9" width="14.625" customWidth="1"/>
-    <col min="10" max="10" width="16.875" customWidth="1"/>
-    <col min="12" max="12" width="19.375" customWidth="1"/>
-    <col min="13" max="13" width="11.875" customWidth="1"/>
-    <col min="15" max="15" width="18.875" customWidth="1"/>
-    <col min="16" max="16" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" customWidth="1"/>
     <col min="17" max="17" width="15.5" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="20" max="20" width="23.625" customWidth="1"/>
+    <col min="20" max="20" width="23.6640625" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
-    <col min="22" max="22" width="15.875" customWidth="1"/>
+    <col min="22" max="22" width="15.83203125" customWidth="1"/>
     <col min="23" max="23" width="23.5" customWidth="1"/>
-    <col min="24" max="24" width="17.375" customWidth="1"/>
-    <col min="26" max="26" width="23.625" customWidth="1"/>
+    <col min="24" max="24" width="17.33203125" customWidth="1"/>
+    <col min="26" max="26" width="23.6640625" customWidth="1"/>
     <col min="30" max="30" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" ht="16" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3711,7 +3719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="16" thickTop="1">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -3795,13 +3803,13 @@
         <v>Amber</v>
       </c>
       <c r="AD2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE2" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3885,13 +3893,13 @@
         <v>Red</v>
       </c>
       <c r="AD3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE3" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -3981,13 +3989,13 @@
         <v>OrangedimSTOCK</v>
       </c>
       <c r="AD4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE4" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -4077,13 +4085,13 @@
         <v>BluebrightSTOCK</v>
       </c>
       <c r="AD5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE5" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -4170,13 +4178,13 @@
         <v>Greenmedium</v>
       </c>
       <c r="AD6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE6" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -4266,13 +4274,13 @@
         <v>GreendimSTOCK</v>
       </c>
       <c r="AD7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE7" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -4362,13 +4370,13 @@
         <v>GreenbrightSTOCK</v>
       </c>
       <c r="AD8" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE8" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -4455,13 +4463,13 @@
         <v>Redmedium</v>
       </c>
       <c r="AD9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE9" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32">
       <c r="A10" t="s">
         <v>126</v>
       </c>
@@ -4551,13 +4559,13 @@
         <v>ReddimSTOCK</v>
       </c>
       <c r="AD10" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE10" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -4647,13 +4655,13 @@
         <v>RedbrightSTOCK</v>
       </c>
       <c r="AD11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE11" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -4740,13 +4748,13 @@
         <v>Redmedium</v>
       </c>
       <c r="AD12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE12" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -4833,13 +4841,13 @@
         <v>Redmedium</v>
       </c>
       <c r="AD13" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE13" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -4929,13 +4937,13 @@
         <v>White, CoolbrightSTOCK</v>
       </c>
       <c r="AD14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE14" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -5025,13 +5033,13 @@
         <v>YellowbrightSTOCK</v>
       </c>
       <c r="AD15" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE15" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32">
       <c r="A16" t="s">
         <v>162</v>
       </c>
@@ -5121,13 +5129,13 @@
         <v>YellowdimSTOCK</v>
       </c>
       <c r="AD16" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE16" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>166</v>
       </c>
@@ -5217,18 +5225,18 @@
         <v>OrangebrightSTOCK</v>
       </c>
       <c r="AD17" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AE17" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5243,37 +5251,37 @@
   <dimension ref="A1:AG46"/>
   <sheetViews>
     <sheetView topLeftCell="AA1" workbookViewId="0">
-      <pane xSplit="14280" topLeftCell="AB1"/>
+      <pane xSplit="14280" topLeftCell="AB1" activePane="topRight"/>
       <selection activeCell="AE47" sqref="AE47:AE48"/>
-      <selection pane="topRight" activeCell="AF5" sqref="AF5:AF46"/>
+      <selection pane="topRight" activeCell="AF5" sqref="AF5:AF34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="3" max="4" width="21.375" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="3" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="4.625" customWidth="1"/>
-    <col min="9" max="10" width="4.875" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="10" width="4.83203125" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="13" width="3.875" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="3.83203125" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="16" width="11.875" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" customWidth="1"/>
     <col min="17" max="17" width="15.5" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="20" max="20" width="23.625" customWidth="1"/>
+    <col min="20" max="20" width="23.6640625" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
-    <col min="22" max="22" width="15.875" customWidth="1"/>
+    <col min="22" max="22" width="15.83203125" customWidth="1"/>
     <col min="23" max="23" width="23.5" customWidth="1"/>
-    <col min="24" max="24" width="17.375" customWidth="1"/>
-    <col min="26" max="27" width="23.625" customWidth="1"/>
-    <col min="31" max="31" width="25.125" customWidth="1"/>
+    <col min="24" max="24" width="17.33203125" customWidth="1"/>
+    <col min="26" max="27" width="23.6640625" customWidth="1"/>
+    <col min="31" max="31" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="16" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5374,7 +5382,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" hidden="1">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -5458,7 +5466,7 @@
         <v>Amber</v>
       </c>
     </row>
-    <row r="3" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" hidden="1">
       <c r="A3" t="s">
         <v>175</v>
       </c>
@@ -5546,7 +5554,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="4" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" hidden="1">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -5634,7 +5642,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="16" thickTop="1">
       <c r="A5" t="s">
         <v>268</v>
       </c>
@@ -5728,13 +5736,13 @@
         <v>BluedimStock</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF5" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -5828,13 +5836,13 @@
         <v>GreendimStock</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF6" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="7" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" hidden="1">
       <c r="A7" t="s">
         <v>226</v>
       </c>
@@ -5922,7 +5930,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="8" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" hidden="1">
       <c r="A8" t="s">
         <v>203</v>
       </c>
@@ -6010,7 +6018,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="9" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" hidden="1">
       <c r="A9" t="s">
         <v>208</v>
       </c>
@@ -6098,7 +6106,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -6192,13 +6200,13 @@
         <v>GreenbrightStock</v>
       </c>
       <c r="AE10" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF10" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="11" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" hidden="1">
       <c r="A11" t="s">
         <v>283</v>
       </c>
@@ -6286,7 +6294,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="12" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" hidden="1">
       <c r="A12" t="s">
         <v>339</v>
       </c>
@@ -6374,7 +6382,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33">
       <c r="A13" t="s">
         <v>187</v>
       </c>
@@ -6468,13 +6476,13 @@
         <v>OrangebrightStock</v>
       </c>
       <c r="AE13" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF13" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33">
       <c r="A14" t="s">
         <v>222</v>
       </c>
@@ -6568,13 +6576,13 @@
         <v>OrangedimStock</v>
       </c>
       <c r="AE14" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF14" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="15" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" hidden="1">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -6662,7 +6670,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="16" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" hidden="1">
       <c r="A16" t="s">
         <v>234</v>
       </c>
@@ -6750,7 +6758,7 @@
         <v>Blue</v>
       </c>
     </row>
-    <row r="17" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" hidden="1">
       <c r="A17" t="s">
         <v>240</v>
       </c>
@@ -6838,7 +6846,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="18" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" hidden="1">
       <c r="A18" t="s">
         <v>250</v>
       </c>
@@ -6926,7 +6934,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="19" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" hidden="1">
       <c r="A19" t="s">
         <v>255</v>
       </c>
@@ -7014,7 +7022,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="20" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" hidden="1">
       <c r="A20" t="s">
         <v>260</v>
       </c>
@@ -7102,7 +7110,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="21" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" hidden="1">
       <c r="A21" t="s">
         <v>265</v>
       </c>
@@ -7190,7 +7198,7 @@
         <v>Blue</v>
       </c>
     </row>
-    <row r="22" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" hidden="1">
       <c r="A22" t="s">
         <v>306</v>
       </c>
@@ -7278,7 +7286,7 @@
         <v>Orange</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32">
       <c r="A23" t="s">
         <v>274</v>
       </c>
@@ -7372,13 +7380,13 @@
         <v>BluebrightStock</v>
       </c>
       <c r="AE23" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF23" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="24" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" hidden="1">
       <c r="A24" t="s">
         <v>318</v>
       </c>
@@ -7466,7 +7474,7 @@
         <v>Orange</v>
       </c>
     </row>
-    <row r="25" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" hidden="1">
       <c r="A25" t="s">
         <v>327</v>
       </c>
@@ -7554,7 +7562,7 @@
         <v>Orange</v>
       </c>
     </row>
-    <row r="26" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" hidden="1">
       <c r="A26" t="s">
         <v>286</v>
       </c>
@@ -7642,7 +7650,7 @@
         <v>Green</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32">
       <c r="A27" t="s">
         <v>291</v>
       </c>
@@ -7736,13 +7744,13 @@
         <v>White, CoolbrightStock</v>
       </c>
       <c r="AE27" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF27" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="28" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" hidden="1">
       <c r="A28" t="s">
         <v>299</v>
       </c>
@@ -7830,7 +7838,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32">
       <c r="A29" t="s">
         <v>211</v>
       </c>
@@ -7924,13 +7932,13 @@
         <v>ReddimStock</v>
       </c>
       <c r="AE29" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF29" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32">
       <c r="A30" t="s">
         <v>311</v>
       </c>
@@ -8024,13 +8032,13 @@
         <v>RedbrightStock</v>
       </c>
       <c r="AE30" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF30" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32">
       <c r="A31" t="s">
         <v>194</v>
       </c>
@@ -8124,13 +8132,13 @@
         <v>YellowbrightStock</v>
       </c>
       <c r="AE31" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF31" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="32" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" hidden="1">
       <c r="A32" t="s">
         <v>215</v>
       </c>
@@ -8218,7 +8226,7 @@
         <v>Yellow</v>
       </c>
     </row>
-    <row r="33" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" hidden="1">
       <c r="A33" t="s">
         <v>323</v>
       </c>
@@ -8306,7 +8314,7 @@
         <v>Yellow</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33">
       <c r="A34" t="s">
         <v>219</v>
       </c>
@@ -8400,13 +8408,13 @@
         <v>YellowdimStock</v>
       </c>
       <c r="AE34" s="9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="AF34" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
-    <row r="35" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" hidden="1">
       <c r="A35" t="s">
         <v>331</v>
       </c>
@@ -8494,7 +8502,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="36" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" hidden="1">
       <c r="A36" t="s">
         <v>314</v>
       </c>
@@ -8582,7 +8590,7 @@
         <v>Yellow</v>
       </c>
     </row>
-    <row r="37" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" hidden="1">
       <c r="A37" t="s">
         <v>342</v>
       </c>
@@ -8670,7 +8678,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="38" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" hidden="1">
       <c r="A38" t="s">
         <v>347</v>
       </c>
@@ -8754,7 +8762,7 @@
         <v>Amber</v>
       </c>
     </row>
-    <row r="39" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" hidden="1">
       <c r="A39" t="s">
         <v>351</v>
       </c>
@@ -8838,7 +8846,7 @@
         <v>Amber</v>
       </c>
     </row>
-    <row r="40" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" hidden="1">
       <c r="A40" t="s">
         <v>211</v>
       </c>
@@ -8922,7 +8930,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="41" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" hidden="1">
       <c r="A41" t="s">
         <v>359</v>
       </c>
@@ -9006,7 +9014,7 @@
         <v>Red</v>
       </c>
     </row>
-    <row r="42" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" hidden="1">
       <c r="A42" t="s">
         <v>362</v>
       </c>
@@ -9090,7 +9098,7 @@
         <v>Blue</v>
       </c>
     </row>
-    <row r="43" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" hidden="1">
       <c r="A43" t="s">
         <v>367</v>
       </c>
@@ -9174,7 +9182,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="44" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" hidden="1">
       <c r="A44" t="s">
         <v>373</v>
       </c>
@@ -9258,7 +9266,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="45" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" hidden="1">
       <c r="A45" t="s">
         <v>381</v>
       </c>
@@ -9342,7 +9350,7 @@
         <v>White, Cool</v>
       </c>
     </row>
-    <row r="46" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" hidden="1">
       <c r="A46" s="2" t="s">
         <v>386</v>
       </c>
@@ -9435,9 +9443,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -9451,37 +9459,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2:AF34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="3" max="4" width="21.375" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="3" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="22.75" customWidth="1"/>
-    <col min="7" max="7" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="4.625" customWidth="1"/>
-    <col min="9" max="10" width="4.875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="10" width="4.83203125" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="13" width="15.125" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" customWidth="1"/>
     <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="16" width="11.875" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" customWidth="1"/>
     <col min="17" max="17" width="15.5" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="20" max="20" width="23.625" customWidth="1"/>
+    <col min="20" max="20" width="23.6640625" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
-    <col min="22" max="22" width="15.875" customWidth="1"/>
+    <col min="22" max="22" width="15.83203125" customWidth="1"/>
     <col min="23" max="23" width="23.5" customWidth="1"/>
-    <col min="24" max="24" width="17.375" customWidth="1"/>
-    <col min="26" max="26" width="23.625" customWidth="1"/>
-    <col min="31" max="31" width="32.75" customWidth="1"/>
-    <col min="32" max="32" width="10.875" customWidth="1"/>
+    <col min="24" max="24" width="17.33203125" customWidth="1"/>
+    <col min="26" max="26" width="23.6640625" customWidth="1"/>
+    <col min="31" max="31" width="32.6640625" customWidth="1"/>
+    <col min="32" max="32" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" ht="16" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9579,7 +9587,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="16" thickTop="1">
       <c r="A2" t="s">
         <v>455</v>
       </c>
@@ -9673,13 +9681,13 @@
         <v>BluebrightStock</v>
       </c>
       <c r="AE2" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF2" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" hidden="1">
       <c r="A3" t="s">
         <v>405</v>
       </c>
@@ -9767,13 +9775,13 @@
         <v>Green</v>
       </c>
       <c r="AE3" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF3" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" hidden="1">
       <c r="A4" t="s">
         <v>405</v>
       </c>
@@ -9861,13 +9869,13 @@
         <v>Green</v>
       </c>
       <c r="AE4" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF4" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" hidden="1">
       <c r="A5" t="s">
         <v>405</v>
       </c>
@@ -9955,13 +9963,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF5" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" hidden="1">
       <c r="A6" t="s">
         <v>405</v>
       </c>
@@ -10049,13 +10057,13 @@
         <v>Red</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF6" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" hidden="1">
       <c r="A7" t="s">
         <v>405</v>
       </c>
@@ -10143,13 +10151,13 @@
         <v>Red</v>
       </c>
       <c r="AE7" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF7" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" hidden="1">
       <c r="A8" t="s">
         <v>455</v>
       </c>
@@ -10237,13 +10245,13 @@
         <v>Blue</v>
       </c>
       <c r="AE8" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF8" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32">
       <c r="A9" t="s">
         <v>397</v>
       </c>
@@ -10337,13 +10345,13 @@
         <v>GreendimStock</v>
       </c>
       <c r="AE9" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF9" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" hidden="1">
       <c r="A10" t="s">
         <v>397</v>
       </c>
@@ -10431,13 +10439,13 @@
         <v>Green</v>
       </c>
       <c r="AE10" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF10" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32">
       <c r="A11" t="s">
         <v>447</v>
       </c>
@@ -10531,13 +10539,13 @@
         <v>GreenbrightStock</v>
       </c>
       <c r="AE11" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF11" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" hidden="1">
       <c r="A12" t="s">
         <v>405</v>
       </c>
@@ -10625,13 +10633,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE12" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF12" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" hidden="1">
       <c r="A13" t="s">
         <v>442</v>
       </c>
@@ -10719,13 +10727,13 @@
         <v>Green</v>
       </c>
       <c r="AE13" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF13" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" hidden="1">
       <c r="A14" t="s">
         <v>442</v>
       </c>
@@ -10813,13 +10821,13 @@
         <v>Green</v>
       </c>
       <c r="AE14" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF14" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" hidden="1">
       <c r="A15" t="s">
         <v>397</v>
       </c>
@@ -10907,13 +10915,13 @@
         <v>Orange</v>
       </c>
       <c r="AE15" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF15" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32">
       <c r="A16" t="s">
         <v>442</v>
       </c>
@@ -11007,13 +11015,13 @@
         <v>OrangedimStock</v>
       </c>
       <c r="AE16" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF16" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32">
       <c r="A17" t="s">
         <v>397</v>
       </c>
@@ -11107,13 +11115,13 @@
         <v>OrangebrightStock</v>
       </c>
       <c r="AE17" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF17" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" hidden="1">
       <c r="A18" t="s">
         <v>455</v>
       </c>
@@ -11201,13 +11209,13 @@
         <v>Blue-Green</v>
       </c>
       <c r="AE18" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF18" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" hidden="1">
       <c r="A19" t="s">
         <v>442</v>
       </c>
@@ -11295,13 +11303,13 @@
         <v>Orange</v>
       </c>
       <c r="AE19" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF19" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" hidden="1">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -11389,13 +11397,13 @@
         <v>Orange</v>
       </c>
       <c r="AE20" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF20" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32">
       <c r="A21" t="s">
         <v>397</v>
       </c>
@@ -11489,13 +11497,13 @@
         <v>ReddimStock</v>
       </c>
       <c r="AE21" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF21" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" hidden="1">
       <c r="A22" t="s">
         <v>397</v>
       </c>
@@ -11583,13 +11591,13 @@
         <v>Red</v>
       </c>
       <c r="AE22" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF22" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" hidden="1">
       <c r="A23" t="s">
         <v>442</v>
       </c>
@@ -11677,13 +11685,13 @@
         <v>Red</v>
       </c>
       <c r="AE23" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF23" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" hidden="1">
       <c r="A24" t="s">
         <v>442</v>
       </c>
@@ -11771,13 +11779,13 @@
         <v>Red</v>
       </c>
       <c r="AE24" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF24" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" hidden="1">
       <c r="A25" t="s">
         <v>489</v>
       </c>
@@ -11865,13 +11873,13 @@
         <v>Red</v>
       </c>
       <c r="AE25" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF25" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32">
       <c r="A26" t="s">
         <v>489</v>
       </c>
@@ -11965,13 +11973,13 @@
         <v>RedbrightStock</v>
       </c>
       <c r="AE26" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF26" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" hidden="1">
       <c r="A27" t="s">
         <v>502</v>
       </c>
@@ -12059,13 +12067,13 @@
         <v>White, Cool</v>
       </c>
       <c r="AE27" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF27" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32">
       <c r="A28" t="s">
         <v>455</v>
       </c>
@@ -12159,13 +12167,13 @@
         <v>White, CoolbrightStock</v>
       </c>
       <c r="AE28" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF28" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" hidden="1">
       <c r="A29" t="s">
         <v>455</v>
       </c>
@@ -12253,13 +12261,13 @@
         <v>White, Cool</v>
       </c>
       <c r="AE29" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF29" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" hidden="1">
       <c r="A30" t="s">
         <v>502</v>
       </c>
@@ -12347,13 +12355,13 @@
         <v>White, Cool</v>
       </c>
       <c r="AE30" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF30" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32">
       <c r="A31" t="s">
         <v>397</v>
       </c>
@@ -12447,13 +12455,13 @@
         <v>YellowdimStock</v>
       </c>
       <c r="AE31" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF31" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" hidden="1">
       <c r="A32" t="s">
         <v>397</v>
       </c>
@@ -12541,13 +12549,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE32" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF32" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" hidden="1">
       <c r="A33" t="s">
         <v>442</v>
       </c>
@@ -12635,13 +12643,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE33" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF33" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32">
       <c r="A34" t="s">
         <v>489</v>
       </c>
@@ -12735,13 +12743,13 @@
         <v>YellowbrightStock</v>
       </c>
       <c r="AE34" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF34" s="5" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" hidden="1">
       <c r="A35" t="s">
         <v>455</v>
       </c>
@@ -12829,13 +12837,13 @@
         <v>Blue-Green</v>
       </c>
       <c r="AE35" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF35" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" hidden="1">
       <c r="A36" t="s">
         <v>541</v>
       </c>
@@ -12923,13 +12931,13 @@
         <v>Green</v>
       </c>
       <c r="AE36" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF36" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" hidden="1">
       <c r="A37" t="s">
         <v>541</v>
       </c>
@@ -13017,13 +13025,13 @@
         <v>Green</v>
       </c>
       <c r="AE37" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF37" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" hidden="1">
       <c r="A38" t="s">
         <v>541</v>
       </c>
@@ -13111,13 +13119,13 @@
         <v>Green</v>
       </c>
       <c r="AE38" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF38" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" hidden="1">
       <c r="A39" t="s">
         <v>541</v>
       </c>
@@ -13205,13 +13213,13 @@
         <v>Green</v>
       </c>
       <c r="AE39" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF39" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" hidden="1">
       <c r="A40" t="s">
         <v>541</v>
       </c>
@@ -13299,13 +13307,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE40" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF40" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" hidden="1">
       <c r="A41" t="s">
         <v>541</v>
       </c>
@@ -13393,13 +13401,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE41" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF41" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" hidden="1">
       <c r="A42" t="s">
         <v>541</v>
       </c>
@@ -13487,13 +13495,13 @@
         <v>Orange</v>
       </c>
       <c r="AE42" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF42" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" hidden="1">
       <c r="A43" t="s">
         <v>541</v>
       </c>
@@ -13581,13 +13589,13 @@
         <v>Orange</v>
       </c>
       <c r="AE43" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF43" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" hidden="1">
       <c r="A44" t="s">
         <v>541</v>
       </c>
@@ -13675,13 +13683,13 @@
         <v>Red</v>
       </c>
       <c r="AE44" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF44" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" hidden="1">
       <c r="A45" t="s">
         <v>442</v>
       </c>
@@ -13769,13 +13777,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE45" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF45" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" hidden="1">
       <c r="A46" t="s">
         <v>541</v>
       </c>
@@ -13863,13 +13871,13 @@
         <v>Red</v>
       </c>
       <c r="AE46" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF46" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" hidden="1">
       <c r="A47" t="s">
         <v>541</v>
       </c>
@@ -13957,13 +13965,13 @@
         <v>Red</v>
       </c>
       <c r="AE47" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF47" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" hidden="1">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -14051,13 +14059,13 @@
         <v>Green</v>
       </c>
       <c r="AE48" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF48" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" hidden="1">
       <c r="A49" t="s">
         <v>589</v>
       </c>
@@ -14145,13 +14153,13 @@
         <v>Green</v>
       </c>
       <c r="AE49" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF49" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:32" hidden="1">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -14239,13 +14247,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE50" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF50" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" hidden="1">
       <c r="A51" t="s">
         <v>405</v>
       </c>
@@ -14333,13 +14341,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE51" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF51" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32" hidden="1">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -14427,13 +14435,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE52" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF52" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:32" hidden="1">
       <c r="A53" t="s">
         <v>405</v>
       </c>
@@ -14521,13 +14529,13 @@
         <v>Orange</v>
       </c>
       <c r="AE53" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF53" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:32" hidden="1">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -14615,13 +14623,13 @@
         <v>Red</v>
       </c>
       <c r="AE54" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF54" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:32" hidden="1">
       <c r="A55" t="s">
         <v>405</v>
       </c>
@@ -14709,13 +14717,13 @@
         <v>Red</v>
       </c>
       <c r="AE55" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF55" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" hidden="1">
       <c r="A56" t="s">
         <v>589</v>
       </c>
@@ -14803,13 +14811,13 @@
         <v>Red</v>
       </c>
       <c r="AE56" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF56" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" hidden="1">
       <c r="A57" t="s">
         <v>489</v>
       </c>
@@ -14897,13 +14905,13 @@
         <v>Orange</v>
       </c>
       <c r="AE57" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF57" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:32" hidden="1">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -14991,13 +14999,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE58" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF58" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:32" hidden="1">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -15085,13 +15093,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE59" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF59" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" hidden="1">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -15179,13 +15187,13 @@
         <v>Orange</v>
       </c>
       <c r="AE60" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF60" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:32" hidden="1">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -15273,13 +15281,13 @@
         <v>Orange</v>
       </c>
       <c r="AE61" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF61" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:32" hidden="1">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -15367,13 +15375,13 @@
         <v>Red</v>
       </c>
       <c r="AE62" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF62" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:32" hidden="1">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -15461,13 +15469,13 @@
         <v>Red</v>
       </c>
       <c r="AE63" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF63" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:32" hidden="1">
       <c r="A64" t="s">
         <v>405</v>
       </c>
@@ -15555,13 +15563,13 @@
         <v>Green</v>
       </c>
       <c r="AE64" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF64" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:32" hidden="1">
       <c r="A65" t="s">
         <v>489</v>
       </c>
@@ -15649,13 +15657,13 @@
         <v>Green</v>
       </c>
       <c r="AE65" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF65" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:32" hidden="1">
       <c r="A66" t="s">
         <v>649</v>
       </c>
@@ -15743,13 +15751,13 @@
         <v>Red</v>
       </c>
       <c r="AE66" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF66" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:32" hidden="1">
       <c r="A67" t="s">
         <v>489</v>
       </c>
@@ -15837,13 +15845,13 @@
         <v>Orange</v>
       </c>
       <c r="AE67" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF67" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:32" hidden="1">
       <c r="A68" t="s">
         <v>489</v>
       </c>
@@ -15931,13 +15939,13 @@
         <v>Yellow</v>
       </c>
       <c r="AE68" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF68" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:32" hidden="1">
       <c r="A69" t="s">
         <v>455</v>
       </c>
@@ -16025,13 +16033,13 @@
         <v>Blue</v>
       </c>
       <c r="AE69" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF69" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:32" hidden="1">
       <c r="A70" t="s">
         <v>455</v>
       </c>
@@ -16119,13 +16127,13 @@
         <v>Blue</v>
       </c>
       <c r="AE70" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF70" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:32" hidden="1">
       <c r="A71" t="s">
         <v>502</v>
       </c>
@@ -16213,13 +16221,13 @@
         <v>White</v>
       </c>
       <c r="AE71" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF71" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:32" hidden="1">
       <c r="A72" t="s">
         <v>455</v>
       </c>
@@ -16307,13 +16315,13 @@
         <v>Blue</v>
       </c>
       <c r="AE72" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF72" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:32" hidden="1">
       <c r="A73" t="s">
         <v>17</v>
       </c>
@@ -16401,13 +16409,13 @@
         <v>White</v>
       </c>
       <c r="AE73" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF73" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:32" hidden="1">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -16495,13 +16503,13 @@
         <v>White</v>
       </c>
       <c r="AE74" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF74" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:32" hidden="1">
       <c r="A75" t="s">
         <v>677</v>
       </c>
@@ -16589,13 +16597,13 @@
         <v>Blue</v>
       </c>
       <c r="AE75" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF75" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:32" hidden="1">
       <c r="A76" t="s">
         <v>677</v>
       </c>
@@ -16683,13 +16691,13 @@
         <v>Green</v>
       </c>
       <c r="AE76" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF76" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:32" hidden="1">
       <c r="A77" t="s">
         <v>502</v>
       </c>
@@ -16777,18 +16785,18 @@
         <v>White, Cool</v>
       </c>
       <c r="AE77" s="9" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AF77" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>